<commit_message>
Fixes for L2SOP pages
Fixed the links for the templates, punctuation fixes, images adjustments.
</commit_message>
<xml_diff>
--- a/input/images/DAK_decision-support logic_template_v2.xlsx
+++ b/input/images/DAK_decision-support logic_template_v2.xlsx
@@ -6,10 +6,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/DigitalAcceleratorKits/Shared Documents/General/Templates and documentation/Templates/L2 SOP GitHub (external only)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WHO\GitHub\smart-ig-starter-kit\input\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{114AFD72-13C1-4EF8-B621-C7689D3CE6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BBA9B26-36CF-4501-B5D9-10DD980E9244}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F41A1C-6F00-44D9-A930-EC3E2D3082B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D729ECD-ABB9-4D06-ACD8-AACFCEA5F9F1}"/>
   </bookViews>
@@ -291,7 +291,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Example of output entries for "System action": recommend repeating the test, recommend additional investigations, recommend updating client's care plan, display additional guidance content. Please check the L2 SOP document, FAQ section, for more examples and clarifications related to how to fill in "System action" output component: https://worldhealthorg.sharepoint.com/:w:/r/sites/DigitalAcceleratorKits/Shared%20Documents/General/Templates%20and%20documentation/Documentation/L2%20SOP%20Wiki%20v2%20(GitHub).docx?d=w7558aaa0660944a2ab870efb22870859&amp;csf=1&amp;web=1&amp;e=LzOeDZ</t>
+Example of output entries for "System action": recommend repeating the test, recommend additional investigations, recommend updating client's care plan, display additional guidance content. Please check the L2 SOP FAQ page, section"Decision-support logic" for more examples and clarifications related to how to fill in "System action" output component: https://smart.who.int/ig-starter-kit/l2_faq.html</t>
         </r>
       </text>
     </comment>
@@ -9440,54 +9440,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc">
-      <UserInfo>
-        <DisplayName>BORG, Sarah Ann</DisplayName>
-        <AccountId>39</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>DUVALL, Susan</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>RATANAPRAYUL, Natschja</DisplayName>
-        <AccountId>7</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>RAMJAUN, Mohammad Shehzaad</DisplayName>
-        <AccountId>44</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MACCHAGIRI, Vineel Chandra</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GAFFIELD, Mary Eluned</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>gndirangu</DisplayName>
-        <AccountId>103</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="73389989-ac93-4f39-a9f3-2949bbf25fcc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A6DDC313EDC9A43B330D8B6305883A5" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5b0342cd22268e5e5d3683a3cff816e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73389989-ac93-4f39-a9f3-2949bbf25fcc" xmlns:ns3="51983ca6-de84-41fa-9a65-1d08ee1009bc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c638d06e48d95e9efa3bb75773f50cd7" ns2:_="" ns3:_="">
     <xsd:import namespace="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
@@ -9742,7 +9694,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9751,18 +9703,55 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD935512-F454-4A53-8449-95D547709634}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
-    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc">
+      <UserInfo>
+        <DisplayName>BORG, Sarah Ann</DisplayName>
+        <AccountId>39</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>DUVALL, Susan</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>RATANAPRAYUL, Natschja</DisplayName>
+        <AccountId>7</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>RAMJAUN, Mohammad Shehzaad</DisplayName>
+        <AccountId>44</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MACCHAGIRI, Vineel Chandra</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GAFFIELD, Mary Eluned</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>gndirangu</DisplayName>
+        <AccountId>103</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="73389989-ac93-4f39-a9f3-2949bbf25fcc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{063694B7-46A6-4CE3-B49D-19C1F7F776B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9781,10 +9770,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45D0A8BA-5511-40DD-A144-F9F7C2155F2F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD935512-F454-4A53-8449-95D547709634}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
+    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>